<commit_message>
updated datasets for income analysis
</commit_message>
<xml_diff>
--- a/merged_datasets/dataset_income_2018-2023.xlsx
+++ b/merged_datasets/dataset_income_2018-2023.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tashasantiago/Desktop/Project_3/merged_datasets/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tashasantiago/Desktop/Data_Science_Certification/project-3/merged_datasets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{64D58D03-E98F-3C46-AC82-E5447B33A000}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD8FBC88-C1E4-3B4B-A281-C4E7F6D0B4D9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="680" yWindow="760" windowWidth="28040" windowHeight="16660" xr2:uid="{B824983F-4401-DC4B-A588-630E88EA66D4}"/>
   </bookViews>
@@ -16,7 +16,20 @@
     <sheet name="dataset_income_2018-2023" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet1" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -1333,8 +1346,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{52BE0851-773F-F24C-8CA7-272232E4FBCD}">
   <dimension ref="A1:BB461"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A432" workbookViewId="0">
-      <selection activeCell="D459" sqref="D459:BB459"/>
+    <sheetView tabSelected="1" topLeftCell="A157" workbookViewId="0">
+      <selection activeCell="C167" sqref="C167"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -27606,204 +27619,204 @@
         <v>102</v>
       </c>
       <c r="C142">
-        <f>C$140*C143/100</f>
-        <v>12488.7</v>
+        <f>C$140*C141/100</f>
+        <v>13380.75</v>
       </c>
       <c r="D142">
-        <f t="shared" ref="D142:BB142" si="60">D$140*D143/100</f>
-        <v>1619.904</v>
+        <f t="shared" ref="D142:BB142" si="60">D$140*D141/100</f>
+        <v>623.04</v>
       </c>
       <c r="E142">
         <f t="shared" si="60"/>
-        <v>15267.972</v>
+        <v>22901.958000000002</v>
       </c>
       <c r="F142">
         <f t="shared" si="60"/>
-        <v>8850.8639999999996</v>
+        <v>7744.5059999999994</v>
       </c>
       <c r="G142">
         <f t="shared" si="60"/>
-        <v>71392.046000000002</v>
+        <v>84372.418000000005</v>
       </c>
       <c r="H142">
         <f t="shared" si="60"/>
-        <v>8934.1360000000004</v>
+        <v>12284.437000000002</v>
       </c>
       <c r="I142">
         <f t="shared" si="60"/>
-        <v>4546.7519999999995</v>
+        <v>5196.2880000000005</v>
       </c>
       <c r="J142">
         <f t="shared" si="60"/>
-        <v>1777.94</v>
+        <v>1600.146</v>
       </c>
       <c r="K142">
         <f t="shared" si="60"/>
-        <v>156.66200000000001</v>
+        <v>704.97900000000004</v>
       </c>
       <c r="L142">
         <f t="shared" si="60"/>
-        <v>47712.665000000001</v>
+        <v>58723.28</v>
       </c>
       <c r="M142">
         <f t="shared" si="60"/>
-        <v>19827.324000000001</v>
+        <v>21629.807999999997</v>
       </c>
       <c r="N142">
         <f t="shared" si="60"/>
-        <v>2320.2399999999998</v>
+        <v>3480.36</v>
       </c>
       <c r="O142">
         <f t="shared" si="60"/>
-        <v>3574.53</v>
+        <v>3931.9830000000006</v>
       </c>
       <c r="P142">
         <f t="shared" si="60"/>
-        <v>18011.207999999999</v>
+        <v>24765.411</v>
       </c>
       <c r="Q142">
         <f t="shared" si="60"/>
-        <v>10992.357</v>
+        <v>13435.103000000001</v>
       </c>
       <c r="R142">
         <f t="shared" si="60"/>
-        <v>5030.8240000000005</v>
+        <v>6288.53</v>
       </c>
       <c r="S142">
         <f t="shared" si="60"/>
-        <v>5144.58</v>
+        <v>5716.2</v>
       </c>
       <c r="T142">
         <f t="shared" si="60"/>
-        <v>12454.02</v>
+        <v>15775.091999999999</v>
       </c>
       <c r="U142">
         <f t="shared" si="60"/>
-        <v>8846.6640000000007</v>
+        <v>10321.108</v>
       </c>
       <c r="V142">
         <f t="shared" si="60"/>
-        <v>2414.3220000000001</v>
+        <v>2682.58</v>
       </c>
       <c r="W142">
         <f t="shared" si="60"/>
-        <v>7359.2329999999993</v>
+        <v>10513.19</v>
       </c>
       <c r="X142">
         <f t="shared" si="60"/>
-        <v>9905.6239999999998</v>
+        <v>12382.03</v>
       </c>
       <c r="Y142">
         <f t="shared" si="60"/>
-        <v>16426.719000000001</v>
+        <v>21902.291999999998</v>
       </c>
       <c r="Z142">
         <f t="shared" si="60"/>
-        <v>6603.4859999999999</v>
+        <v>7704.0669999999991</v>
       </c>
       <c r="AA142">
         <f t="shared" si="60"/>
-        <v>7703.6480000000001</v>
+        <v>8185.1260000000002</v>
       </c>
       <c r="AB142">
         <f t="shared" si="60"/>
-        <v>12766.094000000001</v>
+        <v>15087.201999999999</v>
       </c>
       <c r="AC142">
         <f t="shared" si="60"/>
-        <v>2777.8270000000002</v>
+        <v>1923.1110000000001</v>
       </c>
       <c r="AD142">
         <f t="shared" si="60"/>
-        <v>3496.8420000000001</v>
+        <v>3108.3040000000001</v>
       </c>
       <c r="AE142">
         <f t="shared" si="60"/>
-        <v>5571.17</v>
+        <v>7090.58</v>
       </c>
       <c r="AF142">
         <f t="shared" si="60"/>
-        <v>1642.0919999999999</v>
+        <v>1915.7739999999999</v>
       </c>
       <c r="AG142">
         <f t="shared" si="60"/>
-        <v>11672.240999999998</v>
+        <v>15007.166999999999</v>
       </c>
       <c r="AH142">
         <f t="shared" si="60"/>
-        <v>7624.6149999999989</v>
+        <v>6298.5950000000003</v>
       </c>
       <c r="AI142">
         <f t="shared" si="60"/>
-        <v>41893.995000000003</v>
+        <v>45116.61</v>
       </c>
       <c r="AJ142">
         <f t="shared" si="60"/>
-        <v>19260.79</v>
+        <v>26965.105999999996</v>
       </c>
       <c r="AK142">
         <f t="shared" si="60"/>
-        <v>911.97</v>
+        <v>1519.95</v>
       </c>
       <c r="AL142">
         <f t="shared" si="60"/>
-        <v>23393.392000000003</v>
+        <v>19140.047999999999</v>
       </c>
       <c r="AM142">
         <f t="shared" si="60"/>
-        <v>9990.9039999999986</v>
+        <v>10704.54</v>
       </c>
       <c r="AN142">
         <f t="shared" si="60"/>
-        <v>5465.6490000000003</v>
+        <v>10150.491</v>
       </c>
       <c r="AO142">
         <f t="shared" si="60"/>
-        <v>21360.168000000001</v>
+        <v>26106.872000000003</v>
       </c>
       <c r="AP142">
         <f t="shared" si="60"/>
-        <v>1078.6559999999999</v>
+        <v>1258.432</v>
       </c>
       <c r="AQ142">
         <f t="shared" si="60"/>
-        <v>9288.7000000000007</v>
+        <v>13004.18</v>
       </c>
       <c r="AR142">
         <f t="shared" si="60"/>
-        <v>1065.204</v>
+        <v>1597.806</v>
       </c>
       <c r="AS142">
         <f t="shared" si="60"/>
-        <v>14023.757000000001</v>
+        <v>19123.305</v>
       </c>
       <c r="AT142">
         <f t="shared" si="60"/>
-        <v>59454.792000000001</v>
+        <v>74318.490000000005</v>
       </c>
       <c r="AU142">
         <f t="shared" si="60"/>
-        <v>5573.25</v>
+        <v>6811.75</v>
       </c>
       <c r="AV142">
         <f t="shared" si="60"/>
-        <v>1089.306</v>
+        <v>1452.4079999999999</v>
       </c>
       <c r="AW142">
         <f t="shared" si="60"/>
-        <v>11134.612999999998</v>
+        <v>15906.59</v>
       </c>
       <c r="AX142">
         <f t="shared" si="60"/>
-        <v>11586.976000000001</v>
+        <v>14483.72</v>
       </c>
       <c r="AY142">
         <f t="shared" si="60"/>
-        <v>4936.2179999999998</v>
+        <v>7756.9140000000007</v>
       </c>
       <c r="AZ142">
         <f t="shared" si="60"/>
-        <v>7980</v>
+        <v>9120</v>
       </c>
       <c r="BA142">
         <f t="shared" si="60"/>
@@ -27811,7 +27824,7 @@
       </c>
       <c r="BB142">
         <f t="shared" si="60"/>
-        <v>38374.931000000004</v>
+        <v>42686.721000000005</v>
       </c>
     </row>
     <row r="143" spans="1:54" x14ac:dyDescent="0.2">
@@ -27986,212 +27999,212 @@
         <v>104</v>
       </c>
       <c r="C144">
-        <f>C$140*C145/100</f>
-        <v>41034.299999999996</v>
+        <f>C$140*C143/100</f>
+        <v>12488.7</v>
       </c>
       <c r="D144">
-        <f t="shared" ref="D144:BB144" si="61">D$140*D145/100</f>
-        <v>2242.944</v>
+        <f t="shared" ref="D144:BB144" si="61">D$140*D143/100</f>
+        <v>1619.904</v>
       </c>
       <c r="E144">
         <f t="shared" si="61"/>
-        <v>45803.916000000005</v>
+        <v>15267.972</v>
       </c>
       <c r="F144">
         <f t="shared" si="61"/>
-        <v>33743.919000000002</v>
+        <v>8850.8639999999996</v>
       </c>
       <c r="G144">
         <f t="shared" si="61"/>
-        <v>233646.69600000003</v>
+        <v>71392.046000000002</v>
       </c>
       <c r="H144">
         <f t="shared" si="61"/>
-        <v>24568.874000000003</v>
+        <v>8934.1360000000004</v>
       </c>
       <c r="I144">
         <f t="shared" si="61"/>
-        <v>14289.792000000001</v>
+        <v>4546.7519999999995</v>
       </c>
       <c r="J144">
         <f t="shared" si="61"/>
-        <v>4978.232</v>
+        <v>1777.94</v>
       </c>
       <c r="K144">
         <f t="shared" si="61"/>
-        <v>626.64800000000002</v>
+        <v>156.66200000000001</v>
       </c>
       <c r="L144">
         <f t="shared" si="61"/>
-        <v>150478.40499999997</v>
+        <v>47712.665000000001</v>
       </c>
       <c r="M144">
         <f t="shared" si="61"/>
-        <v>64889.424000000006</v>
+        <v>19827.324000000001</v>
       </c>
       <c r="N144">
         <f t="shared" si="61"/>
-        <v>7192.7440000000006</v>
+        <v>2320.2399999999998</v>
       </c>
       <c r="O144">
         <f t="shared" si="61"/>
-        <v>16442.838</v>
+        <v>3574.53</v>
       </c>
       <c r="P144">
         <f t="shared" si="61"/>
-        <v>60787.827000000005</v>
+        <v>18011.207999999999</v>
       </c>
       <c r="Q144">
         <f t="shared" si="61"/>
-        <v>34198.443999999996</v>
+        <v>10992.357</v>
       </c>
       <c r="R144">
         <f t="shared" si="61"/>
-        <v>16979.031000000003</v>
+        <v>5030.8240000000005</v>
       </c>
       <c r="S144">
         <f t="shared" si="61"/>
-        <v>16576.98</v>
+        <v>5144.58</v>
       </c>
       <c r="T144">
         <f t="shared" si="61"/>
-        <v>37362.06</v>
+        <v>12454.02</v>
       </c>
       <c r="U144">
         <f t="shared" si="61"/>
-        <v>39809.988000000005</v>
+        <v>8846.6640000000007</v>
       </c>
       <c r="V144">
         <f t="shared" si="61"/>
-        <v>9657.2880000000005</v>
+        <v>2414.3220000000001</v>
       </c>
       <c r="W144">
         <f t="shared" si="61"/>
-        <v>18923.741999999998</v>
+        <v>7359.2329999999993</v>
       </c>
       <c r="X144">
         <f t="shared" si="61"/>
-        <v>24764.06</v>
+        <v>9905.6239999999998</v>
       </c>
       <c r="Y144">
         <f t="shared" si="61"/>
-        <v>58406.112000000001</v>
+        <v>16426.719000000001</v>
       </c>
       <c r="Z144">
         <f t="shared" si="61"/>
-        <v>22011.62</v>
+        <v>6603.4859999999999</v>
       </c>
       <c r="AA144">
         <f t="shared" si="61"/>
-        <v>26481.29</v>
+        <v>7703.6480000000001</v>
       </c>
       <c r="AB144">
         <f t="shared" si="61"/>
-        <v>39458.836000000003</v>
+        <v>12766.094000000001</v>
       </c>
       <c r="AC144">
         <f t="shared" si="61"/>
-        <v>8760.8389999999999</v>
+        <v>2777.8270000000002</v>
       </c>
       <c r="AD144">
         <f t="shared" si="61"/>
-        <v>10490.526000000002</v>
+        <v>3496.8420000000001</v>
       </c>
       <c r="AE144">
         <f t="shared" si="61"/>
-        <v>17219.98</v>
+        <v>5571.17</v>
       </c>
       <c r="AF144">
         <f t="shared" si="61"/>
-        <v>4926.2760000000007</v>
+        <v>1642.0919999999999</v>
       </c>
       <c r="AG144">
         <f t="shared" si="61"/>
-        <v>36684.186000000002</v>
+        <v>11672.240999999998</v>
       </c>
       <c r="AH144">
         <f t="shared" si="61"/>
-        <v>21216.32</v>
+        <v>7624.6149999999989</v>
       </c>
       <c r="AI144">
         <f t="shared" si="61"/>
-        <v>112791.52499999999</v>
+        <v>41893.995000000003</v>
       </c>
       <c r="AJ144">
         <f t="shared" si="61"/>
-        <v>73191.001999999993</v>
+        <v>19260.79</v>
       </c>
       <c r="AK144">
         <f t="shared" si="61"/>
-        <v>5015.835</v>
+        <v>911.97</v>
       </c>
       <c r="AL144">
         <f t="shared" si="61"/>
-        <v>57420.144</v>
+        <v>23393.392000000003</v>
       </c>
       <c r="AM144">
         <f t="shared" si="61"/>
-        <v>29259.075999999997</v>
+        <v>9990.9039999999986</v>
       </c>
       <c r="AN144">
         <f t="shared" si="61"/>
-        <v>22643.402999999998</v>
+        <v>5465.6490000000003</v>
       </c>
       <c r="AO144">
         <f t="shared" si="61"/>
-        <v>64080.504000000001</v>
+        <v>21360.168000000001</v>
       </c>
       <c r="AP144">
         <f t="shared" si="61"/>
-        <v>4853.9520000000002</v>
+        <v>1078.6559999999999</v>
       </c>
       <c r="AQ144">
         <f t="shared" si="61"/>
-        <v>32510.45</v>
+        <v>9288.7000000000007</v>
       </c>
       <c r="AR144">
         <f t="shared" si="61"/>
-        <v>5503.5540000000001</v>
+        <v>1065.204</v>
       </c>
       <c r="AS144">
         <f t="shared" si="61"/>
-        <v>52270.366999999991</v>
+        <v>14023.757000000001</v>
       </c>
       <c r="AT144">
         <f t="shared" si="61"/>
-        <v>203137.20599999998</v>
+        <v>59454.792000000001</v>
       </c>
       <c r="AU144">
         <f t="shared" si="61"/>
-        <v>17339</v>
+        <v>5573.25</v>
       </c>
       <c r="AV144">
         <f t="shared" si="61"/>
-        <v>3146.884</v>
+        <v>1089.306</v>
       </c>
       <c r="AW144">
         <f t="shared" si="61"/>
-        <v>38175.815999999999</v>
+        <v>11134.612999999998</v>
       </c>
       <c r="AX144">
         <f t="shared" si="61"/>
-        <v>34760.928</v>
+        <v>11586.976000000001</v>
       </c>
       <c r="AY144">
         <f t="shared" si="61"/>
-        <v>16924.175999999999</v>
+        <v>4936.2179999999998</v>
       </c>
       <c r="AZ144">
         <f t="shared" si="61"/>
-        <v>29640</v>
+        <v>7980</v>
       </c>
       <c r="BA144">
         <f t="shared" si="61"/>
-        <v>4324.0749999999998</v>
+        <v>1235.45</v>
       </c>
       <c r="BB144">
         <f t="shared" si="61"/>
-        <v>79768.115000000005</v>
+        <v>38374.931000000004</v>
       </c>
     </row>
     <row r="145" spans="1:54" x14ac:dyDescent="0.2">
@@ -28366,212 +28379,212 @@
         <v>106</v>
       </c>
       <c r="C146">
-        <f>C$140*C147/100</f>
-        <v>59767.35</v>
+        <f>C$140*C145/100</f>
+        <v>41034.299999999996</v>
       </c>
       <c r="D146">
-        <f t="shared" ref="D146:BB146" si="62">D$140*D147/100</f>
-        <v>4485.8879999999999</v>
+        <f t="shared" ref="D146:BB146" si="62">D$140*D145/100</f>
+        <v>2242.944</v>
       </c>
       <c r="E146">
         <f t="shared" si="62"/>
-        <v>67433.543000000005</v>
+        <v>45803.916000000005</v>
       </c>
       <c r="F146">
         <f t="shared" si="62"/>
-        <v>44807.498999999996</v>
+        <v>33743.919000000002</v>
       </c>
       <c r="G146">
         <f t="shared" si="62"/>
-        <v>298548.55599999998</v>
+        <v>233646.69600000003</v>
       </c>
       <c r="H146">
         <f t="shared" si="62"/>
-        <v>41320.379000000001</v>
+        <v>24568.874000000003</v>
       </c>
       <c r="I146">
         <f t="shared" si="62"/>
-        <v>17537.472000000002</v>
+        <v>14289.792000000001</v>
       </c>
       <c r="J146">
         <f t="shared" si="62"/>
-        <v>7111.76</v>
+        <v>4978.232</v>
       </c>
       <c r="K146">
         <f t="shared" si="62"/>
-        <v>1096.634</v>
+        <v>626.64800000000002</v>
       </c>
       <c r="L146">
         <f t="shared" si="62"/>
-        <v>220212.3</v>
+        <v>150478.40499999997</v>
       </c>
       <c r="M146">
         <f t="shared" si="62"/>
-        <v>99136.62</v>
+        <v>64889.424000000006</v>
       </c>
       <c r="N146">
         <f t="shared" si="62"/>
-        <v>8816.9120000000003</v>
+        <v>7192.7440000000006</v>
       </c>
       <c r="O146">
         <f t="shared" si="62"/>
-        <v>20017.367999999999</v>
+        <v>16442.838</v>
       </c>
       <c r="P146">
         <f t="shared" si="62"/>
-        <v>92307.440999999992</v>
+        <v>60787.827000000005</v>
       </c>
       <c r="Q146">
         <f t="shared" si="62"/>
-        <v>61068.65</v>
+        <v>34198.443999999996</v>
       </c>
       <c r="R146">
         <f t="shared" si="62"/>
-        <v>27040.679</v>
+        <v>16979.031000000003</v>
       </c>
       <c r="S146">
         <f t="shared" si="62"/>
-        <v>26294.52</v>
+        <v>16576.98</v>
       </c>
       <c r="T146">
         <f t="shared" si="62"/>
-        <v>54797.687999999995</v>
+        <v>37362.06</v>
       </c>
       <c r="U146">
         <f t="shared" si="62"/>
-        <v>47182.207999999999</v>
+        <v>39809.988000000005</v>
       </c>
       <c r="V146">
         <f t="shared" si="62"/>
-        <v>14217.673999999999</v>
+        <v>9657.2880000000005</v>
       </c>
       <c r="W146">
         <f t="shared" si="62"/>
-        <v>27334.293999999998</v>
+        <v>18923.741999999998</v>
       </c>
       <c r="X146">
         <f t="shared" si="62"/>
-        <v>35907.886999999995</v>
+        <v>24764.06</v>
       </c>
       <c r="Y146">
         <f t="shared" si="62"/>
-        <v>91259.55</v>
+        <v>58406.112000000001</v>
       </c>
       <c r="Z146">
         <f t="shared" si="62"/>
-        <v>37419.754000000001</v>
+        <v>22011.62</v>
       </c>
       <c r="AA146">
         <f t="shared" si="62"/>
-        <v>32740.504000000001</v>
+        <v>26481.29</v>
       </c>
       <c r="AB146">
         <f t="shared" si="62"/>
-        <v>61509.362000000001</v>
+        <v>39458.836000000003</v>
       </c>
       <c r="AC146">
         <f t="shared" si="62"/>
-        <v>11111.308000000001</v>
+        <v>8760.8389999999999</v>
       </c>
       <c r="AD146">
         <f t="shared" si="62"/>
-        <v>16707.133999999998</v>
+        <v>10490.526000000002</v>
       </c>
       <c r="AE146">
         <f t="shared" si="62"/>
-        <v>27855.85</v>
+        <v>17219.98</v>
       </c>
       <c r="AF146">
         <f t="shared" si="62"/>
-        <v>9031.5059999999994</v>
+        <v>4926.2760000000007</v>
       </c>
       <c r="AG146">
         <f t="shared" si="62"/>
-        <v>56693.741999999998</v>
+        <v>36684.186000000002</v>
       </c>
       <c r="AH146">
         <f t="shared" si="62"/>
-        <v>24531.37</v>
+        <v>21216.32</v>
       </c>
       <c r="AI146">
         <f t="shared" si="62"/>
-        <v>132127.21499999997</v>
+        <v>112791.52499999999</v>
       </c>
       <c r="AJ146">
         <f t="shared" si="62"/>
-        <v>111712.58199999999</v>
+        <v>73191.001999999993</v>
       </c>
       <c r="AK146">
         <f t="shared" si="62"/>
-        <v>5319.8249999999998</v>
+        <v>5015.835</v>
       </c>
       <c r="AL146">
         <f t="shared" si="62"/>
-        <v>106333.6</v>
+        <v>57420.144</v>
       </c>
       <c r="AM146">
         <f t="shared" si="62"/>
-        <v>46386.34</v>
+        <v>29259.075999999997</v>
       </c>
       <c r="AN146">
         <f t="shared" si="62"/>
-        <v>37478.736000000004</v>
+        <v>22643.402999999998</v>
       </c>
       <c r="AO146">
         <f t="shared" si="62"/>
-        <v>106800.84</v>
+        <v>64080.504000000001</v>
       </c>
       <c r="AP146">
         <f t="shared" si="62"/>
-        <v>5573.0559999999996</v>
+        <v>4853.9520000000002</v>
       </c>
       <c r="AQ146">
         <f t="shared" si="62"/>
-        <v>50158.98</v>
+        <v>32510.45</v>
       </c>
       <c r="AR146">
         <f t="shared" si="62"/>
-        <v>8699.1660000000011</v>
+        <v>5503.5540000000001</v>
       </c>
       <c r="AS146">
         <f t="shared" si="62"/>
-        <v>81592.768000000011</v>
+        <v>52270.366999999991</v>
       </c>
       <c r="AT146">
         <f t="shared" si="62"/>
-        <v>262591.99800000002</v>
+        <v>203137.20599999998</v>
       </c>
       <c r="AU146">
         <f t="shared" si="62"/>
-        <v>26627.75</v>
+        <v>17339</v>
       </c>
       <c r="AV146">
         <f t="shared" si="62"/>
-        <v>4962.3939999999993</v>
+        <v>3146.884</v>
       </c>
       <c r="AW146">
         <f t="shared" si="62"/>
-        <v>62035.700999999994</v>
+        <v>38175.815999999999</v>
       </c>
       <c r="AX146">
         <f t="shared" si="62"/>
-        <v>47796.275999999998</v>
+        <v>34760.928</v>
       </c>
       <c r="AY146">
         <f t="shared" si="62"/>
-        <v>27501.786</v>
+        <v>16924.175999999999</v>
       </c>
       <c r="AZ146">
         <f t="shared" si="62"/>
-        <v>46740</v>
+        <v>29640</v>
       </c>
       <c r="BA146">
         <f t="shared" si="62"/>
-        <v>5930.16</v>
+        <v>4324.0749999999998</v>
       </c>
       <c r="BB146">
         <f t="shared" si="62"/>
-        <v>62089.776000000005</v>
+        <v>79768.115000000005</v>
       </c>
     </row>
     <row r="147" spans="1:54" x14ac:dyDescent="0.2">
@@ -28746,212 +28759,212 @@
         <v>108</v>
       </c>
       <c r="C148">
-        <f>C$140*C149/100</f>
-        <v>101693.7</v>
+        <f>C$140*C147/100</f>
+        <v>59767.35</v>
       </c>
       <c r="D148">
-        <f t="shared" ref="D148:BB148" si="63">D$140*D149/100</f>
-        <v>9594.8159999999989</v>
+        <f t="shared" ref="D148:BB148" si="63">D$140*D147/100</f>
+        <v>4485.8879999999999</v>
       </c>
       <c r="E148">
         <f t="shared" si="63"/>
-        <v>134867.08600000001</v>
+        <v>67433.543000000005</v>
       </c>
       <c r="F148">
         <f t="shared" si="63"/>
-        <v>66381.48</v>
+        <v>44807.498999999996</v>
       </c>
       <c r="G148">
         <f t="shared" si="63"/>
-        <v>499744.32200000004</v>
+        <v>298548.55599999998</v>
       </c>
       <c r="H148">
         <f t="shared" si="63"/>
-        <v>79290.456999999995</v>
+        <v>41320.379000000001</v>
       </c>
       <c r="I148">
         <f t="shared" si="63"/>
-        <v>39621.695999999996</v>
+        <v>17537.472000000002</v>
       </c>
       <c r="J148">
         <f t="shared" si="63"/>
-        <v>14934.696000000002</v>
+        <v>7111.76</v>
       </c>
       <c r="K148">
         <f t="shared" si="63"/>
-        <v>2584.9229999999998</v>
+        <v>1096.634</v>
       </c>
       <c r="L148">
         <f t="shared" si="63"/>
-        <v>400052.34499999997</v>
+        <v>220212.3</v>
       </c>
       <c r="M148">
         <f t="shared" si="63"/>
-        <v>165828.52799999999</v>
+        <v>99136.62</v>
       </c>
       <c r="N148">
         <f t="shared" si="63"/>
-        <v>14385.488000000001</v>
+        <v>8816.9120000000003</v>
       </c>
       <c r="O148">
         <f t="shared" si="63"/>
-        <v>39319.83</v>
+        <v>20017.367999999999</v>
       </c>
       <c r="P148">
         <f t="shared" si="63"/>
-        <v>182363.48099999997</v>
+        <v>92307.440999999992</v>
       </c>
       <c r="Q148">
         <f t="shared" si="63"/>
-        <v>122137.3</v>
+        <v>61068.65</v>
       </c>
       <c r="R148">
         <f t="shared" si="63"/>
-        <v>60369.887999999999</v>
+        <v>27040.679</v>
       </c>
       <c r="S148">
         <f t="shared" si="63"/>
-        <v>56018.76</v>
+        <v>26294.52</v>
       </c>
       <c r="T148">
         <f t="shared" si="63"/>
-        <v>97971.624000000011</v>
+        <v>54797.687999999995</v>
       </c>
       <c r="U148">
         <f t="shared" si="63"/>
-        <v>73722.2</v>
+        <v>47182.207999999999</v>
       </c>
       <c r="V148">
         <f t="shared" si="63"/>
-        <v>26021.025999999998</v>
+        <v>14217.673999999999</v>
       </c>
       <c r="W148">
         <f t="shared" si="63"/>
-        <v>57822.544999999998</v>
+        <v>27334.293999999998</v>
       </c>
       <c r="X148">
         <f t="shared" si="63"/>
-        <v>73053.976999999999</v>
+        <v>35907.886999999995</v>
       </c>
       <c r="Y148">
         <f t="shared" si="63"/>
-        <v>180693.90900000001</v>
+        <v>91259.55</v>
       </c>
       <c r="Z148">
         <f t="shared" si="63"/>
-        <v>74839.508000000002</v>
+        <v>37419.754000000001</v>
       </c>
       <c r="AA148">
         <f t="shared" si="63"/>
-        <v>63555.095999999998</v>
+        <v>32740.504000000001</v>
       </c>
       <c r="AB148">
         <f t="shared" si="63"/>
-        <v>124179.27799999999</v>
+        <v>61509.362000000001</v>
       </c>
       <c r="AC148">
         <f t="shared" si="63"/>
-        <v>25427.800999999999</v>
+        <v>11111.308000000001</v>
       </c>
       <c r="AD148">
         <f t="shared" si="63"/>
-        <v>36911.11</v>
+        <v>16707.133999999998</v>
       </c>
       <c r="AE148">
         <f t="shared" si="63"/>
-        <v>50647</v>
+        <v>27855.85</v>
       </c>
       <c r="AF148">
         <f t="shared" si="63"/>
-        <v>21894.560000000001</v>
+        <v>9031.5059999999994</v>
       </c>
       <c r="AG148">
         <f t="shared" si="63"/>
-        <v>100047.78</v>
+        <v>56693.741999999998</v>
       </c>
       <c r="AH148">
         <f t="shared" si="63"/>
-        <v>33150.5</v>
+        <v>24531.37</v>
       </c>
       <c r="AI148">
         <f t="shared" si="63"/>
-        <v>248141.35500000001</v>
+        <v>132127.21499999997</v>
       </c>
       <c r="AJ148">
         <f t="shared" si="63"/>
-        <v>204164.37399999998</v>
+        <v>111712.58199999999</v>
       </c>
       <c r="AK148">
         <f t="shared" si="63"/>
-        <v>12007.605</v>
+        <v>5319.8249999999998</v>
       </c>
       <c r="AL148">
         <f t="shared" si="63"/>
-        <v>202033.84</v>
+        <v>106333.6</v>
       </c>
       <c r="AM148">
         <f t="shared" si="63"/>
-        <v>79927.231999999989</v>
+        <v>46386.34</v>
       </c>
       <c r="AN148">
         <f t="shared" si="63"/>
-        <v>70272.63</v>
+        <v>37478.736000000004</v>
       </c>
       <c r="AO148">
         <f t="shared" si="63"/>
-        <v>215975.03200000001</v>
+        <v>106800.84</v>
       </c>
       <c r="AP148">
         <f t="shared" si="63"/>
-        <v>13123.648000000001</v>
+        <v>5573.0559999999996</v>
       </c>
       <c r="AQ148">
         <f t="shared" si="63"/>
-        <v>100317.96</v>
+        <v>50158.98</v>
       </c>
       <c r="AR148">
         <f t="shared" si="63"/>
-        <v>15622.992000000002</v>
+        <v>8699.1660000000011</v>
       </c>
       <c r="AS148">
         <f t="shared" si="63"/>
-        <v>140237.57</v>
+        <v>81592.768000000011</v>
       </c>
       <c r="AT148">
         <f t="shared" si="63"/>
-        <v>470683.77</v>
+        <v>262591.99800000002</v>
       </c>
       <c r="AU148">
         <f t="shared" si="63"/>
-        <v>47063</v>
+        <v>26627.75</v>
       </c>
       <c r="AV148">
         <f t="shared" si="63"/>
-        <v>9561.6860000000015</v>
+        <v>4962.3939999999993</v>
       </c>
       <c r="AW148">
         <f t="shared" si="63"/>
-        <v>114527.448</v>
+        <v>62035.700999999994</v>
       </c>
       <c r="AX148">
         <f t="shared" si="63"/>
-        <v>99937.668000000005</v>
+        <v>47796.275999999998</v>
       </c>
       <c r="AY148">
         <f t="shared" si="63"/>
-        <v>50419.941000000006</v>
+        <v>27501.786</v>
       </c>
       <c r="AZ148">
         <f t="shared" si="63"/>
-        <v>98040</v>
+        <v>46740</v>
       </c>
       <c r="BA148">
         <f t="shared" si="63"/>
-        <v>10007.145</v>
+        <v>5930.16</v>
       </c>
       <c r="BB148">
         <f t="shared" si="63"/>
-        <v>68988.639999999999</v>
+        <v>62089.776000000005</v>
       </c>
     </row>
     <row r="149" spans="1:54" x14ac:dyDescent="0.2">
@@ -29126,212 +29139,212 @@
         <v>110</v>
       </c>
       <c r="C150">
-        <f>C$140*C151/100</f>
-        <v>177517.95</v>
+        <f>C$140*C149/100</f>
+        <v>101693.7</v>
       </c>
       <c r="D150">
-        <f t="shared" ref="D150:BB150" si="64">D$140*D151/100</f>
-        <v>19812.671999999999</v>
+        <f t="shared" ref="D150:BB150" si="64">D$140*D149/100</f>
+        <v>9594.8159999999989</v>
       </c>
       <c r="E150">
         <f t="shared" si="64"/>
-        <v>232836.573</v>
+        <v>134867.08600000001</v>
       </c>
       <c r="F150">
         <f t="shared" si="64"/>
-        <v>119486.664</v>
+        <v>66381.48</v>
       </c>
       <c r="G150">
         <f t="shared" si="64"/>
-        <v>889155.48199999984</v>
+        <v>499744.32200000004</v>
       </c>
       <c r="H150">
         <f t="shared" si="64"/>
-        <v>169748.58399999997</v>
+        <v>79290.456999999995</v>
       </c>
       <c r="I150">
         <f t="shared" si="64"/>
-        <v>82491.071999999986</v>
+        <v>39621.695999999996</v>
       </c>
       <c r="J150">
         <f t="shared" si="64"/>
-        <v>28091.452000000001</v>
+        <v>14934.696000000002</v>
       </c>
       <c r="K150">
         <f t="shared" si="64"/>
-        <v>5169.8459999999995</v>
+        <v>2584.9229999999998</v>
       </c>
       <c r="L150">
         <f t="shared" si="64"/>
-        <v>697338.95</v>
+        <v>400052.34499999997</v>
       </c>
       <c r="M150">
         <f t="shared" si="64"/>
-        <v>326249.60400000005</v>
+        <v>165828.52799999999</v>
       </c>
       <c r="N150">
         <f t="shared" si="64"/>
-        <v>32947.407999999996</v>
+        <v>14385.488000000001</v>
       </c>
       <c r="O150">
         <f t="shared" si="64"/>
-        <v>77209.848000000013</v>
+        <v>39319.83</v>
       </c>
       <c r="P150">
         <f t="shared" si="64"/>
-        <v>337710.15</v>
+        <v>182363.48099999997</v>
       </c>
       <c r="Q150">
         <f t="shared" si="64"/>
-        <v>252824.21099999998</v>
+        <v>122137.3</v>
       </c>
       <c r="R150">
         <f t="shared" si="64"/>
-        <v>124512.894</v>
+        <v>60369.887999999999</v>
       </c>
       <c r="S150">
         <f t="shared" si="64"/>
-        <v>110322.66</v>
+        <v>56018.76</v>
       </c>
       <c r="T150">
         <f t="shared" si="64"/>
-        <v>168544.40400000001</v>
+        <v>97971.624000000011</v>
       </c>
       <c r="U150">
         <f t="shared" si="64"/>
-        <v>126802.18400000001</v>
+        <v>73722.2</v>
       </c>
       <c r="V150">
         <f t="shared" si="64"/>
-        <v>53115.084000000003</v>
+        <v>26021.025999999998</v>
       </c>
       <c r="W150">
         <f t="shared" si="64"/>
-        <v>124055.64200000001</v>
+        <v>57822.544999999998</v>
       </c>
       <c r="X150">
         <f t="shared" si="64"/>
-        <v>133725.924</v>
+        <v>73053.976999999999</v>
       </c>
       <c r="Y150">
         <f t="shared" si="64"/>
-        <v>344961.09899999999</v>
+        <v>180693.90900000001</v>
       </c>
       <c r="Z150">
         <f t="shared" si="64"/>
-        <v>166187.731</v>
+        <v>74839.508000000002</v>
       </c>
       <c r="AA150">
         <f t="shared" si="64"/>
-        <v>103036.29199999999</v>
+        <v>63555.095999999998</v>
       </c>
       <c r="AB150">
         <f t="shared" si="64"/>
-        <v>230950.24599999998</v>
+        <v>124179.27799999999</v>
       </c>
       <c r="AC150">
         <f t="shared" si="64"/>
-        <v>44231.553</v>
+        <v>25427.800999999999</v>
       </c>
       <c r="AD150">
         <f t="shared" si="64"/>
-        <v>75376.371999999988</v>
+        <v>36911.11</v>
       </c>
       <c r="AE150">
         <f t="shared" si="64"/>
-        <v>93190.48</v>
+        <v>50647</v>
       </c>
       <c r="AF150">
         <f t="shared" si="64"/>
-        <v>38589.161999999997</v>
+        <v>21894.560000000001</v>
       </c>
       <c r="AG150">
         <f t="shared" si="64"/>
-        <v>195093.17099999997</v>
+        <v>100047.78</v>
       </c>
       <c r="AH150">
         <f t="shared" si="64"/>
-        <v>63980.464999999997</v>
+        <v>33150.5</v>
       </c>
       <c r="AI150">
         <f t="shared" si="64"/>
-        <v>451166.1</v>
+        <v>248141.35500000001</v>
       </c>
       <c r="AJ150">
         <f t="shared" si="64"/>
-        <v>364028.93099999992</v>
+        <v>204164.37399999998</v>
       </c>
       <c r="AK150">
         <f t="shared" si="64"/>
-        <v>24775.185000000001</v>
+        <v>12007.605</v>
       </c>
       <c r="AL150">
         <f t="shared" si="64"/>
-        <v>412574.36799999996</v>
+        <v>202033.84</v>
       </c>
       <c r="AM150">
         <f t="shared" si="64"/>
-        <v>142727.20000000001</v>
+        <v>79927.231999999989</v>
       </c>
       <c r="AN150">
         <f t="shared" si="64"/>
-        <v>135860.41799999998</v>
+        <v>70272.63</v>
       </c>
       <c r="AO150">
         <f t="shared" si="64"/>
-        <v>408216.54399999999</v>
+        <v>215975.03200000001</v>
       </c>
       <c r="AP150">
         <f t="shared" si="64"/>
-        <v>27865.279999999999</v>
+        <v>13123.648000000001</v>
       </c>
       <c r="AQ150">
         <f t="shared" si="64"/>
-        <v>182058.52</v>
+        <v>100317.96</v>
       </c>
       <c r="AR150">
         <f t="shared" si="64"/>
-        <v>37637.207999999999</v>
+        <v>15622.992000000002</v>
       </c>
       <c r="AS150">
         <f t="shared" si="64"/>
-        <v>248602.965</v>
+        <v>140237.57</v>
       </c>
       <c r="AT150">
         <f t="shared" si="64"/>
-        <v>817503.39</v>
+        <v>470683.77</v>
       </c>
       <c r="AU150">
         <f t="shared" si="64"/>
-        <v>114561.25</v>
+        <v>47063</v>
       </c>
       <c r="AV150">
         <f t="shared" si="64"/>
-        <v>22149.222000000002</v>
+        <v>9561.6860000000015</v>
       </c>
       <c r="AW150">
         <f t="shared" si="64"/>
-        <v>225873.57799999998</v>
+        <v>114527.448</v>
       </c>
       <c r="AX150">
         <f t="shared" si="64"/>
-        <v>215807.42800000001</v>
+        <v>99937.668000000005</v>
       </c>
       <c r="AY150">
         <f t="shared" si="64"/>
-        <v>74043.27</v>
+        <v>50419.941000000006</v>
       </c>
       <c r="AZ150">
         <f t="shared" si="64"/>
-        <v>212040</v>
+        <v>98040</v>
       </c>
       <c r="BA150">
         <f t="shared" si="64"/>
-        <v>25450.27</v>
+        <v>10007.145</v>
       </c>
       <c r="BB150">
         <f t="shared" si="64"/>
-        <v>65970.387000000002</v>
+        <v>68988.639999999999</v>
       </c>
     </row>
     <row r="151" spans="1:54" x14ac:dyDescent="0.2">
@@ -29506,56 +29519,56 @@
         <v>112</v>
       </c>
       <c r="C152">
-        <f>C$140*C153/100</f>
-        <v>144512.1</v>
+        <f>C$140*C151/100</f>
+        <v>177517.95</v>
       </c>
       <c r="D152">
-        <f t="shared" ref="D152:BB152" si="65">D$140*D153/100</f>
-        <v>18192.768</v>
+        <f t="shared" ref="D152:BB152" si="65">D$140*D151/100</f>
+        <v>19812.671999999999</v>
       </c>
       <c r="E152">
         <f t="shared" si="65"/>
-        <v>211206.94600000003</v>
+        <v>232836.573</v>
       </c>
       <c r="F152">
         <f t="shared" si="65"/>
-        <v>91274.535000000003</v>
+        <v>119486.664</v>
       </c>
       <c r="G152">
         <f t="shared" si="65"/>
-        <v>856704.55199999991</v>
+        <v>889155.48199999984</v>
       </c>
       <c r="H152">
         <f t="shared" si="65"/>
-        <v>170865.35100000002</v>
+        <v>169748.58399999997</v>
       </c>
       <c r="I152">
         <f t="shared" si="65"/>
-        <v>84439.679999999993</v>
+        <v>82491.071999999986</v>
       </c>
       <c r="J152">
         <f t="shared" si="65"/>
-        <v>29691.597999999998</v>
+        <v>28091.452000000001</v>
       </c>
       <c r="K152">
         <f t="shared" si="65"/>
-        <v>6031.487000000001</v>
+        <v>5169.8459999999995</v>
       </c>
       <c r="L152">
         <f t="shared" si="65"/>
-        <v>598243.41500000004</v>
+        <v>697338.95</v>
       </c>
       <c r="M152">
         <f t="shared" si="65"/>
-        <v>282989.98799999995</v>
+        <v>326249.60400000005</v>
       </c>
       <c r="N152">
         <f t="shared" si="65"/>
-        <v>35267.648000000001</v>
+        <v>32947.407999999996</v>
       </c>
       <c r="O152">
         <f t="shared" si="65"/>
-        <v>65056.445999999996</v>
+        <v>77209.848000000013</v>
       </c>
       <c r="P152">
         <f t="shared" si="65"/>
@@ -29563,123 +29576,123 @@
       </c>
       <c r="Q152">
         <f t="shared" si="65"/>
-        <v>219847.14</v>
+        <v>252824.21099999998</v>
       </c>
       <c r="R152">
         <f t="shared" si="65"/>
-        <v>120110.92300000001</v>
+        <v>124512.894</v>
       </c>
       <c r="S152">
         <f t="shared" si="65"/>
-        <v>101748.36</v>
+        <v>110322.66</v>
       </c>
       <c r="T152">
         <f t="shared" si="65"/>
-        <v>146127.16800000001</v>
+        <v>168544.40400000001</v>
       </c>
       <c r="U152">
         <f t="shared" si="65"/>
-        <v>126064.96200000001</v>
+        <v>126802.18400000001</v>
       </c>
       <c r="V152">
         <f t="shared" si="65"/>
-        <v>50432.504000000001</v>
+        <v>53115.084000000003</v>
       </c>
       <c r="W152">
         <f t="shared" si="65"/>
-        <v>133517.51299999998</v>
+        <v>124055.64200000001</v>
       </c>
       <c r="X152">
         <f t="shared" si="65"/>
-        <v>147346.15700000001</v>
+        <v>133725.924</v>
       </c>
       <c r="Y152">
         <f t="shared" si="65"/>
-        <v>315758.04300000001</v>
+        <v>344961.09899999999</v>
       </c>
       <c r="Z152">
         <f t="shared" si="65"/>
-        <v>184897.60800000001</v>
+        <v>166187.731</v>
       </c>
       <c r="AA152">
         <f t="shared" si="65"/>
-        <v>79925.348000000013</v>
+        <v>103036.29199999999</v>
       </c>
       <c r="AB152">
         <f t="shared" si="65"/>
-        <v>203096.95</v>
+        <v>230950.24599999998</v>
       </c>
       <c r="AC152">
         <f t="shared" si="65"/>
-        <v>37821.182999999997</v>
+        <v>44231.553</v>
       </c>
       <c r="AD152">
         <f t="shared" si="65"/>
-        <v>73045.144</v>
+        <v>75376.371999999988</v>
       </c>
       <c r="AE152">
         <f t="shared" si="65"/>
-        <v>88125.78</v>
+        <v>93190.48</v>
       </c>
       <c r="AF152">
         <f t="shared" si="65"/>
-        <v>43789.120000000003</v>
+        <v>38589.161999999997</v>
       </c>
       <c r="AG152">
         <f t="shared" si="65"/>
-        <v>203430.48599999998</v>
+        <v>195093.17099999997</v>
       </c>
       <c r="AH152">
         <f t="shared" si="65"/>
-        <v>53703.81</v>
+        <v>63980.464999999997</v>
       </c>
       <c r="AI152">
         <f t="shared" si="65"/>
-        <v>431830.41</v>
+        <v>451166.1</v>
       </c>
       <c r="AJ152">
         <f t="shared" si="65"/>
-        <v>325507.35099999997</v>
+        <v>364028.93099999992</v>
       </c>
       <c r="AK152">
         <f t="shared" si="65"/>
-        <v>27207.105</v>
+        <v>24775.185000000001</v>
       </c>
       <c r="AL152">
         <f t="shared" si="65"/>
-        <v>374294.27200000006</v>
+        <v>412574.36799999996</v>
       </c>
       <c r="AM152">
         <f t="shared" si="65"/>
-        <v>124172.66399999999</v>
+        <v>142727.20000000001</v>
       </c>
       <c r="AN152">
         <f t="shared" si="65"/>
-        <v>129613.96200000001</v>
+        <v>135860.41799999998</v>
       </c>
       <c r="AO152">
         <f t="shared" si="65"/>
-        <v>401096.48799999995</v>
+        <v>408216.54399999999</v>
       </c>
       <c r="AP152">
         <f t="shared" si="65"/>
-        <v>29303.488000000001</v>
+        <v>27865.279999999999</v>
       </c>
       <c r="AQ152">
         <f t="shared" si="65"/>
-        <v>158836.77000000002</v>
+        <v>182058.52</v>
       </c>
       <c r="AR152">
         <f t="shared" si="65"/>
-        <v>34619.129999999997</v>
+        <v>37637.207999999999</v>
       </c>
       <c r="AS152">
         <f t="shared" si="65"/>
-        <v>221830.33799999996</v>
+        <v>248602.965</v>
       </c>
       <c r="AT152">
         <f t="shared" si="65"/>
-        <v>758048.598</v>
+        <v>817503.39</v>
       </c>
       <c r="AU152">
         <f t="shared" si="65"/>
@@ -29687,31 +29700,31 @@
       </c>
       <c r="AV152">
         <f t="shared" si="65"/>
-        <v>21059.915999999997</v>
+        <v>22149.222000000002</v>
       </c>
       <c r="AW152">
         <f t="shared" si="65"/>
-        <v>230645.55499999999</v>
+        <v>225873.57799999998</v>
       </c>
       <c r="AX152">
         <f t="shared" si="65"/>
-        <v>224497.66</v>
+        <v>215807.42800000001</v>
       </c>
       <c r="AY152">
         <f t="shared" si="65"/>
-        <v>60644.963999999993</v>
+        <v>74043.27</v>
       </c>
       <c r="AZ152">
         <f t="shared" si="65"/>
-        <v>210900</v>
+        <v>212040</v>
       </c>
       <c r="BA152">
         <f t="shared" si="65"/>
-        <v>24338.365000000002</v>
+        <v>25450.27</v>
       </c>
       <c r="BB152">
         <f t="shared" si="65"/>
-        <v>31044.888000000003</v>
+        <v>65970.387000000002</v>
       </c>
     </row>
     <row r="153" spans="1:54" x14ac:dyDescent="0.2">
@@ -29886,212 +29899,212 @@
         <v>114</v>
       </c>
       <c r="C154">
-        <f>C$140*C155/100</f>
-        <v>192682.8</v>
+        <f>C$140*C153/100</f>
+        <v>144512.1</v>
       </c>
       <c r="D154">
-        <f t="shared" ref="D154:BB154" si="66">D$140*D155/100</f>
-        <v>30155.136000000002</v>
+        <f t="shared" ref="D154:BB154" si="66">D$140*D153/100</f>
+        <v>18192.768</v>
       </c>
       <c r="E154">
         <f t="shared" si="66"/>
-        <v>278640.489</v>
+        <v>211206.94600000003</v>
       </c>
       <c r="F154">
         <f t="shared" si="66"/>
-        <v>105657.189</v>
+        <v>91274.535000000003</v>
       </c>
       <c r="G154">
         <f t="shared" si="66"/>
-        <v>1369429.2460000003</v>
+        <v>856704.55199999991</v>
       </c>
       <c r="H154">
         <f t="shared" si="66"/>
-        <v>276958.21600000001</v>
+        <v>170865.35100000002</v>
       </c>
       <c r="I154">
         <f t="shared" si="66"/>
-        <v>150692.35199999998</v>
+        <v>84439.679999999993</v>
       </c>
       <c r="J154">
         <f t="shared" si="66"/>
-        <v>44804.087999999996</v>
+        <v>29691.597999999998</v>
       </c>
       <c r="K154">
         <f t="shared" si="66"/>
-        <v>13551.263000000001</v>
+        <v>6031.487000000001</v>
       </c>
       <c r="L154">
         <f t="shared" si="66"/>
-        <v>745051.61499999999</v>
+        <v>598243.41500000004</v>
       </c>
       <c r="M154">
         <f t="shared" si="66"/>
-        <v>401953.93200000003</v>
+        <v>282989.98799999995</v>
       </c>
       <c r="N154">
         <f t="shared" si="66"/>
-        <v>59398.144</v>
+        <v>35267.648000000001</v>
       </c>
       <c r="O154">
         <f t="shared" si="66"/>
-        <v>75780.035999999993</v>
+        <v>65056.445999999996</v>
       </c>
       <c r="P154">
         <f t="shared" si="66"/>
-        <v>556096.0469999999</v>
+        <v>337710.15</v>
       </c>
       <c r="Q154">
         <f t="shared" si="66"/>
-        <v>293129.52</v>
+        <v>219847.14</v>
       </c>
       <c r="R154">
         <f t="shared" si="66"/>
-        <v>154697.83800000002</v>
+        <v>120110.92300000001</v>
       </c>
       <c r="S154">
         <f t="shared" si="66"/>
-        <v>136617.18</v>
+        <v>101748.36</v>
       </c>
       <c r="T154">
         <f t="shared" si="66"/>
-        <v>170204.94</v>
+        <v>146127.16800000001</v>
       </c>
       <c r="U154">
         <f t="shared" si="66"/>
-        <v>161451.61799999999</v>
+        <v>126064.96200000001</v>
       </c>
       <c r="V154">
         <f t="shared" si="66"/>
-        <v>61699.34</v>
+        <v>50432.504000000001</v>
       </c>
       <c r="W154">
         <f t="shared" si="66"/>
-        <v>256521.83599999998</v>
+        <v>133517.51299999998</v>
       </c>
       <c r="X154">
         <f t="shared" si="66"/>
-        <v>292215.908</v>
+        <v>147346.15700000001</v>
       </c>
       <c r="Y154">
         <f t="shared" si="66"/>
-        <v>417968.739</v>
+        <v>315758.04300000001</v>
       </c>
       <c r="Z154">
         <f t="shared" si="66"/>
-        <v>292754.54600000003</v>
+        <v>184897.60800000001</v>
       </c>
       <c r="AA154">
         <f t="shared" si="66"/>
-        <v>93406.731999999989</v>
+        <v>79925.348000000013</v>
       </c>
       <c r="AB154">
         <f t="shared" si="66"/>
-        <v>264606.31199999998</v>
+        <v>203096.95</v>
       </c>
       <c r="AC154">
         <f t="shared" si="66"/>
-        <v>47864.095999999998</v>
+        <v>37821.182999999997</v>
       </c>
       <c r="AD154">
         <f t="shared" si="66"/>
-        <v>95191.81</v>
+        <v>73045.144</v>
       </c>
       <c r="AE154">
         <f t="shared" si="66"/>
-        <v>113955.75</v>
+        <v>88125.78</v>
       </c>
       <c r="AF154">
         <f t="shared" si="66"/>
-        <v>70062.592000000004</v>
+        <v>43789.120000000003</v>
       </c>
       <c r="AG154">
         <f t="shared" si="66"/>
-        <v>380181.56400000001</v>
+        <v>203430.48599999998</v>
       </c>
       <c r="AH154">
         <f t="shared" si="66"/>
-        <v>64643.474999999999</v>
+        <v>53703.81</v>
       </c>
       <c r="AI154">
         <f t="shared" si="66"/>
-        <v>686416.995</v>
+        <v>431830.41</v>
       </c>
       <c r="AJ154">
         <f t="shared" si="66"/>
-        <v>414106.98499999999</v>
+        <v>325507.35099999997</v>
       </c>
       <c r="AK154">
         <f t="shared" si="66"/>
-        <v>42710.595000000001</v>
+        <v>27207.105</v>
       </c>
       <c r="AL154">
         <f t="shared" si="66"/>
-        <v>499767.92</v>
+        <v>374294.27200000006</v>
       </c>
       <c r="AM154">
         <f t="shared" si="66"/>
-        <v>152718.10399999999</v>
+        <v>124172.66399999999</v>
       </c>
       <c r="AN154">
         <f t="shared" si="66"/>
-        <v>186612.87300000002</v>
+        <v>129613.96200000001</v>
       </c>
       <c r="AO154">
         <f t="shared" si="66"/>
-        <v>557737.72</v>
+        <v>401096.48799999995</v>
       </c>
       <c r="AP154">
         <f t="shared" si="66"/>
-        <v>45303.552000000003</v>
+        <v>29303.488000000001</v>
       </c>
       <c r="AQ154">
         <f t="shared" si="66"/>
-        <v>201564.79</v>
+        <v>158836.77000000002</v>
       </c>
       <c r="AR154">
         <f t="shared" si="66"/>
-        <v>43673.364000000001</v>
+        <v>34619.129999999997</v>
       </c>
       <c r="AS154">
         <f t="shared" si="66"/>
-        <v>267726.27</v>
+        <v>221830.33799999996</v>
       </c>
       <c r="AT154">
         <f t="shared" si="66"/>
-        <v>1099913.652</v>
+        <v>758048.598</v>
       </c>
       <c r="AU154">
         <f t="shared" si="66"/>
-        <v>157289.5</v>
+        <v>114561.25</v>
       </c>
       <c r="AV154">
         <f t="shared" si="66"/>
-        <v>32074.01</v>
+        <v>21059.915999999997</v>
       </c>
       <c r="AW154">
         <f t="shared" si="66"/>
-        <v>362670.25200000004</v>
+        <v>230645.55499999999</v>
       </c>
       <c r="AX154">
         <f t="shared" si="66"/>
-        <v>344712.53600000002</v>
+        <v>224497.66</v>
       </c>
       <c r="AY154">
         <f t="shared" si="66"/>
-        <v>69107.051999999996</v>
+        <v>60644.963999999993</v>
       </c>
       <c r="AZ154">
         <f t="shared" si="66"/>
-        <v>299820</v>
+        <v>210900</v>
       </c>
       <c r="BA154">
         <f t="shared" si="66"/>
-        <v>30021.435000000001</v>
+        <v>24338.365000000002</v>
       </c>
       <c r="BB154">
         <f t="shared" si="66"/>
-        <v>25439.561000000002</v>
+        <v>31044.888000000003</v>
       </c>
     </row>
     <row r="155" spans="1:54" x14ac:dyDescent="0.2">
@@ -30266,212 +30279,212 @@
         <v>116</v>
       </c>
       <c r="C156">
-        <f>C$140*C157/100</f>
-        <v>78500.400000000009</v>
+        <f>C$140*C155/100</f>
+        <v>192682.8</v>
       </c>
       <c r="D156">
-        <f t="shared" ref="D156:BB156" si="67">D$140*D157/100</f>
-        <v>19563.455999999998</v>
+        <f t="shared" ref="D156:BB156" si="67">D$140*D155/100</f>
+        <v>30155.136000000002</v>
       </c>
       <c r="E156">
         <f t="shared" si="67"/>
-        <v>125960.769</v>
+        <v>278640.489</v>
       </c>
       <c r="F156">
         <f t="shared" si="67"/>
-        <v>37616.171999999999</v>
+        <v>105657.189</v>
       </c>
       <c r="G156">
         <f t="shared" si="67"/>
-        <v>843724.18</v>
+        <v>1369429.2460000003</v>
       </c>
       <c r="H156">
         <f t="shared" si="67"/>
-        <v>152997.079</v>
+        <v>276958.21600000001</v>
       </c>
       <c r="I156">
         <f t="shared" si="67"/>
-        <v>98079.936000000002</v>
+        <v>150692.35199999998</v>
       </c>
       <c r="J156">
         <f t="shared" si="67"/>
-        <v>23113.22</v>
+        <v>44804.087999999996</v>
       </c>
       <c r="K156">
         <f t="shared" si="67"/>
-        <v>12689.621999999999</v>
+        <v>13551.263000000001</v>
       </c>
       <c r="L156">
         <f t="shared" si="67"/>
-        <v>337658.86</v>
+        <v>745051.61499999999</v>
       </c>
       <c r="M156">
         <f t="shared" si="67"/>
-        <v>191063.30399999997</v>
+        <v>401953.93200000003</v>
       </c>
       <c r="N156">
         <f t="shared" si="67"/>
-        <v>32715.383999999998</v>
+        <v>59398.144</v>
       </c>
       <c r="O156">
         <f t="shared" si="67"/>
-        <v>28953.692999999999</v>
+        <v>75780.035999999993</v>
       </c>
       <c r="P156">
         <f t="shared" si="67"/>
-        <v>288179.32799999998</v>
+        <v>556096.0469999999</v>
       </c>
       <c r="Q156">
         <f t="shared" si="67"/>
-        <v>114809.06200000001</v>
+        <v>293129.52</v>
       </c>
       <c r="R156">
         <f t="shared" si="67"/>
-        <v>59741.035000000003</v>
+        <v>154697.83800000002</v>
       </c>
       <c r="S156">
         <f t="shared" si="67"/>
-        <v>54303.9</v>
+        <v>136617.18</v>
       </c>
       <c r="T156">
         <f t="shared" si="67"/>
-        <v>66421.440000000002</v>
+        <v>170204.94</v>
       </c>
       <c r="U156">
         <f t="shared" si="67"/>
-        <v>71510.534</v>
+        <v>161451.61799999999</v>
       </c>
       <c r="V156">
         <f t="shared" si="67"/>
-        <v>23874.962000000003</v>
+        <v>61699.34</v>
       </c>
       <c r="W156">
         <f t="shared" si="67"/>
-        <v>168211.04</v>
+        <v>256521.83599999998</v>
       </c>
       <c r="X156">
         <f t="shared" si="67"/>
-        <v>204303.495</v>
+        <v>292215.908</v>
       </c>
       <c r="Y156">
         <f t="shared" si="67"/>
-        <v>189819.86400000003</v>
+        <v>417968.739</v>
       </c>
       <c r="Z156">
         <f t="shared" si="67"/>
-        <v>149679.016</v>
+        <v>292754.54600000003</v>
       </c>
       <c r="AA156">
         <f t="shared" si="67"/>
-        <v>37555.284</v>
+        <v>93406.731999999989</v>
       </c>
       <c r="AB156">
         <f t="shared" si="67"/>
-        <v>105610.414</v>
+        <v>264606.31199999998</v>
       </c>
       <c r="AC156">
         <f t="shared" si="67"/>
-        <v>17307.999</v>
+        <v>47864.095999999998</v>
       </c>
       <c r="AD156">
         <f t="shared" si="67"/>
-        <v>40019.414000000004</v>
+        <v>95191.81</v>
       </c>
       <c r="AE156">
         <f t="shared" si="67"/>
-        <v>48114.65</v>
+        <v>113955.75</v>
       </c>
       <c r="AF156">
         <f t="shared" si="67"/>
-        <v>38315.480000000003</v>
+        <v>70062.592000000004</v>
       </c>
       <c r="AG156">
         <f t="shared" si="67"/>
-        <v>253454.37599999999</v>
+        <v>380181.56400000001</v>
       </c>
       <c r="AH156">
         <f t="shared" si="67"/>
-        <v>30166.955000000002</v>
+        <v>64643.474999999999</v>
       </c>
       <c r="AI156">
         <f t="shared" si="67"/>
-        <v>422162.565</v>
+        <v>686416.995</v>
       </c>
       <c r="AJ156">
         <f t="shared" si="67"/>
-        <v>181051.42600000001</v>
+        <v>414106.98499999999</v>
       </c>
       <c r="AK156">
         <f t="shared" si="67"/>
-        <v>15351.495000000001</v>
+        <v>42710.595000000001</v>
       </c>
       <c r="AL156">
         <f t="shared" si="67"/>
-        <v>219047.21600000001</v>
+        <v>499767.92</v>
       </c>
       <c r="AM156">
         <f t="shared" si="67"/>
-        <v>60659.06</v>
+        <v>152718.10399999999</v>
       </c>
       <c r="AN156">
         <f t="shared" si="67"/>
-        <v>90573.611999999994</v>
+        <v>186612.87300000002</v>
       </c>
       <c r="AO156">
         <f t="shared" si="67"/>
-        <v>270562.12800000003</v>
+        <v>557737.72</v>
       </c>
       <c r="AP156">
         <f t="shared" si="67"/>
-        <v>25528.191999999995</v>
+        <v>45303.552000000003</v>
       </c>
       <c r="AQ156">
         <f t="shared" si="67"/>
-        <v>92887</v>
+        <v>201564.79</v>
       </c>
       <c r="AR156">
         <f t="shared" si="67"/>
-        <v>15622.992000000002</v>
+        <v>43673.364000000001</v>
       </c>
       <c r="AS156">
         <f t="shared" si="67"/>
-        <v>109640.28199999999</v>
+        <v>267726.27</v>
       </c>
       <c r="AT156">
         <f t="shared" si="67"/>
-        <v>554911.39199999999</v>
+        <v>1099913.652</v>
       </c>
       <c r="AU156">
         <f t="shared" si="67"/>
-        <v>68117.5</v>
+        <v>157289.5</v>
       </c>
       <c r="AV156">
         <f t="shared" si="67"/>
-        <v>13313.74</v>
+        <v>32074.01</v>
       </c>
       <c r="AW156">
         <f t="shared" si="67"/>
-        <v>214738.965</v>
+        <v>362670.25200000004</v>
       </c>
       <c r="AX156">
         <f t="shared" si="67"/>
-        <v>196978.592</v>
+        <v>344712.53600000002</v>
       </c>
       <c r="AY156">
         <f t="shared" si="67"/>
-        <v>21507.806999999997</v>
+        <v>69107.051999999996</v>
       </c>
       <c r="AZ156">
         <f t="shared" si="67"/>
-        <v>121980</v>
+        <v>299820</v>
       </c>
       <c r="BA156">
         <f t="shared" si="67"/>
-        <v>11613.23</v>
+        <v>30021.435000000001</v>
       </c>
       <c r="BB156">
         <f t="shared" si="67"/>
-        <v>7330.0429999999997</v>
+        <v>25439.561000000002</v>
       </c>
     </row>
     <row r="157" spans="1:54" x14ac:dyDescent="0.2">
@@ -30646,16 +30659,16 @@
         <v>118</v>
       </c>
       <c r="C158">
-        <f>C$140*C159/100</f>
-        <v>70471.95</v>
+        <f>C$140*C157/100</f>
+        <v>78500.400000000009</v>
       </c>
       <c r="D158">
-        <f t="shared" ref="D158:BB158" si="68">D$140*D159/100</f>
-        <v>18441.984</v>
+        <f t="shared" ref="D158:BB158" si="68">D$140*D157/100</f>
+        <v>19563.455999999998</v>
       </c>
       <c r="E158">
         <f t="shared" si="68"/>
-        <v>138684.079</v>
+        <v>125960.769</v>
       </c>
       <c r="F158">
         <f t="shared" si="68"/>
@@ -30663,59 +30676,59 @@
       </c>
       <c r="G158">
         <f t="shared" si="68"/>
-        <v>1349958.6880000001</v>
+        <v>843724.18</v>
       </c>
       <c r="H158">
         <f t="shared" si="68"/>
-        <v>182033.02100000001</v>
+        <v>152997.079</v>
       </c>
       <c r="I158">
         <f t="shared" si="68"/>
-        <v>151991.424</v>
+        <v>98079.936000000002</v>
       </c>
       <c r="J158">
         <f t="shared" si="68"/>
-        <v>21868.662</v>
+        <v>23113.22</v>
       </c>
       <c r="K158">
         <f t="shared" si="68"/>
-        <v>35718.936000000002</v>
+        <v>12689.621999999999</v>
       </c>
       <c r="L158">
         <f t="shared" si="68"/>
-        <v>414733.16499999998</v>
+        <v>337658.86</v>
       </c>
       <c r="M158">
         <f t="shared" si="68"/>
-        <v>228915.46799999996</v>
+        <v>191063.30399999997</v>
       </c>
       <c r="N158">
         <f t="shared" si="68"/>
-        <v>35731.696000000004</v>
+        <v>32715.383999999998</v>
       </c>
       <c r="O158">
         <f t="shared" si="68"/>
-        <v>27166.428</v>
+        <v>28953.692999999999</v>
       </c>
       <c r="P158">
         <f t="shared" si="68"/>
-        <v>355721.35800000007</v>
+        <v>288179.32799999998</v>
       </c>
       <c r="Q158">
         <f t="shared" si="68"/>
-        <v>100152.586</v>
+        <v>114809.06200000001</v>
       </c>
       <c r="R158">
         <f t="shared" si="68"/>
-        <v>54081.358</v>
+        <v>59741.035000000003</v>
       </c>
       <c r="S158">
         <f t="shared" si="68"/>
-        <v>59448.480000000003</v>
+        <v>54303.9</v>
       </c>
       <c r="T158">
         <f t="shared" si="68"/>
-        <v>59779.296000000002</v>
+        <v>66421.440000000002</v>
       </c>
       <c r="U158">
         <f t="shared" si="68"/>
@@ -30723,135 +30736,135 @@
       </c>
       <c r="V158">
         <f t="shared" si="68"/>
-        <v>24143.22</v>
+        <v>23874.962000000003</v>
       </c>
       <c r="W158">
         <f t="shared" si="68"/>
-        <v>247059.965</v>
+        <v>168211.04</v>
       </c>
       <c r="X158">
         <f t="shared" si="68"/>
-        <v>304597.93800000002</v>
+        <v>204303.495</v>
       </c>
       <c r="Y158">
         <f t="shared" si="68"/>
-        <v>187994.67300000001</v>
+        <v>189819.86400000003</v>
       </c>
       <c r="Z158">
         <f t="shared" si="68"/>
-        <v>158483.66399999999</v>
+        <v>149679.016</v>
       </c>
       <c r="AA158">
         <f t="shared" si="68"/>
-        <v>28407.202000000001</v>
+        <v>37555.284</v>
       </c>
       <c r="AB158">
         <f t="shared" si="68"/>
-        <v>104449.86</v>
+        <v>105610.414</v>
       </c>
       <c r="AC158">
         <f t="shared" si="68"/>
-        <v>16239.603999999999</v>
+        <v>17307.999</v>
       </c>
       <c r="AD158">
         <f t="shared" si="68"/>
-        <v>34579.882000000005</v>
+        <v>40019.414000000004</v>
       </c>
       <c r="AE158">
         <f t="shared" si="68"/>
-        <v>55205.23</v>
+        <v>48114.65</v>
       </c>
       <c r="AF158">
         <f t="shared" si="68"/>
-        <v>43789.120000000003</v>
+        <v>38315.480000000003</v>
       </c>
       <c r="AG158">
         <f t="shared" si="68"/>
-        <v>415198.28699999995</v>
+        <v>253454.37599999999</v>
       </c>
       <c r="AH158">
         <f t="shared" si="68"/>
-        <v>26188.895</v>
+        <v>30166.955000000002</v>
       </c>
       <c r="AI158">
         <f t="shared" si="68"/>
-        <v>654190.84499999997</v>
+        <v>422162.565</v>
       </c>
       <c r="AJ158">
         <f t="shared" si="68"/>
-        <v>208016.53200000004</v>
+        <v>181051.42600000001</v>
       </c>
       <c r="AK158">
         <f t="shared" si="68"/>
-        <v>17175.435000000001</v>
+        <v>15351.495000000001</v>
       </c>
       <c r="AL158">
         <f t="shared" si="68"/>
-        <v>212667.2</v>
+        <v>219047.21600000001</v>
       </c>
       <c r="AM158">
         <f t="shared" si="68"/>
-        <v>57090.879999999997</v>
+        <v>60659.06</v>
       </c>
       <c r="AN158">
         <f t="shared" si="68"/>
-        <v>91354.419000000009</v>
+        <v>90573.611999999994</v>
       </c>
       <c r="AO158">
         <f t="shared" si="68"/>
-        <v>303789.05600000004</v>
+        <v>270562.12800000003</v>
       </c>
       <c r="AP158">
         <f t="shared" si="68"/>
-        <v>26067.52</v>
+        <v>25528.191999999995</v>
       </c>
       <c r="AQ158">
         <f t="shared" si="68"/>
-        <v>88242.65</v>
+        <v>92887</v>
       </c>
       <c r="AR158">
         <f t="shared" si="68"/>
-        <v>13670.118</v>
+        <v>15622.992000000002</v>
       </c>
       <c r="AS158">
         <f t="shared" si="68"/>
-        <v>118564.49100000001</v>
+        <v>109640.28199999999</v>
       </c>
       <c r="AT158">
         <f t="shared" si="68"/>
-        <v>658957.27800000005</v>
+        <v>554911.39199999999</v>
       </c>
       <c r="AU158">
         <f t="shared" si="68"/>
-        <v>61305.75</v>
+        <v>68117.5</v>
       </c>
       <c r="AV158">
         <f t="shared" si="68"/>
-        <v>12224.433999999999</v>
+        <v>13313.74</v>
       </c>
       <c r="AW158">
         <f t="shared" si="68"/>
-        <v>313359.82299999997</v>
+        <v>214738.965</v>
       </c>
       <c r="AX158">
         <f t="shared" si="68"/>
-        <v>259258.58799999996</v>
+        <v>196978.592</v>
       </c>
       <c r="AY158">
         <f t="shared" si="68"/>
-        <v>20450.045999999998</v>
+        <v>21507.806999999997</v>
       </c>
       <c r="AZ158">
         <f t="shared" si="68"/>
-        <v>104880</v>
+        <v>121980</v>
       </c>
       <c r="BA158">
         <f t="shared" si="68"/>
-        <v>9389.42</v>
+        <v>11613.23</v>
       </c>
       <c r="BB158">
         <f t="shared" si="68"/>
-        <v>9054.759</v>
+        <v>7330.0429999999997</v>
       </c>
     </row>
     <row r="159" spans="1:54" x14ac:dyDescent="0.2">
@@ -31026,212 +31039,212 @@
         <v>120</v>
       </c>
       <c r="C160">
-        <f>C$140*C161/100</f>
-        <v>726066256.5</v>
+        <f>C$140*C159/100</f>
+        <v>70471.95</v>
       </c>
       <c r="D160">
-        <f t="shared" ref="D160:BB160" si="69">D$140*D161/100</f>
-        <v>132141799.68000001</v>
+        <f t="shared" ref="D160:BB160" si="69">D$140*D159/100</f>
+        <v>18441.984</v>
       </c>
       <c r="E160">
         <f t="shared" si="69"/>
-        <v>1115936073.48</v>
+        <v>138684.079</v>
       </c>
       <c r="F160">
         <f t="shared" si="69"/>
-        <v>408223974.83999997</v>
+        <v>37616.171999999999</v>
       </c>
       <c r="G160">
         <f t="shared" si="69"/>
-        <v>7084751939.46</v>
+        <v>1349958.6880000001</v>
       </c>
       <c r="H160">
         <f t="shared" si="69"/>
-        <v>1201574285.98</v>
+        <v>182033.02100000001</v>
       </c>
       <c r="I160">
         <f t="shared" si="69"/>
-        <v>797506796.15999997</v>
+        <v>151991.424</v>
       </c>
       <c r="J160">
         <f t="shared" si="69"/>
-        <v>178876765.46000001</v>
+        <v>21868.662</v>
       </c>
       <c r="K160">
         <f t="shared" si="69"/>
-        <v>144793286.88</v>
+        <v>35718.936000000002</v>
       </c>
       <c r="L160">
         <f t="shared" si="69"/>
-        <v>3110792353.9000001</v>
+        <v>414733.16499999998</v>
       </c>
       <c r="M160">
         <f t="shared" si="69"/>
-        <v>1670199699.24</v>
+        <v>228915.46799999996</v>
       </c>
       <c r="N160">
         <f t="shared" si="69"/>
-        <v>251017484.63999999</v>
+        <v>35731.696000000004</v>
       </c>
       <c r="O160">
         <f t="shared" si="69"/>
-        <v>289708507.44</v>
+        <v>27166.428</v>
       </c>
       <c r="P160">
         <f t="shared" si="69"/>
-        <v>2356744052.79</v>
+        <v>355721.35800000007</v>
       </c>
       <c r="Q160">
         <f t="shared" si="69"/>
-        <v>1067480002</v>
+        <v>100152.586</v>
       </c>
       <c r="R160">
         <f t="shared" si="69"/>
-        <v>567112212.46000004</v>
+        <v>54081.358</v>
       </c>
       <c r="S160">
         <f t="shared" si="69"/>
-        <v>515384024.39999998</v>
+        <v>59448.480000000003</v>
       </c>
       <c r="T160">
         <f t="shared" si="69"/>
-        <v>653645088.36000001</v>
+        <v>59779.296000000002</v>
       </c>
       <c r="U160">
         <f t="shared" si="69"/>
-        <v>638279435.38</v>
+        <v>71510.534</v>
       </c>
       <c r="V160">
         <f t="shared" si="69"/>
-        <v>233041089.75999999</v>
+        <v>24143.22</v>
       </c>
       <c r="W160">
         <f t="shared" si="69"/>
-        <v>1327668712.3399999</v>
+        <v>247059.965</v>
       </c>
       <c r="X160">
         <f t="shared" si="69"/>
-        <v>1607880887.6800001</v>
+        <v>304597.93800000002</v>
       </c>
       <c r="Y160">
         <f t="shared" si="69"/>
-        <v>1642817915.28</v>
+        <v>187994.67300000001</v>
       </c>
       <c r="Z160">
         <f t="shared" si="69"/>
-        <v>1171854625.5599999</v>
+        <v>158483.66399999999</v>
       </c>
       <c r="AA160">
         <f t="shared" si="69"/>
-        <v>359413697.44</v>
+        <v>28407.202000000001</v>
       </c>
       <c r="AB160">
         <f t="shared" si="69"/>
-        <v>1003055216.66</v>
+        <v>104449.86</v>
       </c>
       <c r="AC160">
         <f t="shared" si="69"/>
-        <v>176522358.69</v>
+        <v>16239.603999999999</v>
       </c>
       <c r="AD160">
         <f t="shared" si="69"/>
-        <v>354024169.45999998</v>
+        <v>34579.882000000005</v>
       </c>
       <c r="AE160">
         <f t="shared" si="69"/>
-        <v>449416154.5</v>
+        <v>55205.23</v>
       </c>
       <c r="AF160">
         <f t="shared" si="69"/>
-        <v>298576114.72000003</v>
+        <v>43789.120000000003</v>
       </c>
       <c r="AG160">
         <f t="shared" si="69"/>
-        <v>2097351636.03</v>
+        <v>415198.28699999995</v>
       </c>
       <c r="AH160">
         <f t="shared" si="69"/>
-        <v>261106598.19999999</v>
+        <v>26188.895</v>
       </c>
       <c r="AI160">
         <f t="shared" si="69"/>
-        <v>3506043989.25</v>
+        <v>654190.84499999997</v>
       </c>
       <c r="AJ160">
         <f t="shared" si="69"/>
-        <v>1680465405.9200001</v>
+        <v>208016.53200000004</v>
       </c>
       <c r="AK160">
         <f t="shared" si="69"/>
-        <v>150181699.65000001</v>
+        <v>17175.435000000001</v>
       </c>
       <c r="AL160">
         <f t="shared" si="69"/>
-        <v>1930635375.04</v>
+        <v>212667.2</v>
       </c>
       <c r="AM160">
         <f t="shared" si="69"/>
-        <v>584774747.48000002</v>
+        <v>57090.879999999997</v>
       </c>
       <c r="AN160">
         <f t="shared" si="69"/>
-        <v>746529572.70000005</v>
+        <v>91354.419000000009</v>
       </c>
       <c r="AO160">
         <f t="shared" si="69"/>
-        <v>2276115768.5599999</v>
+        <v>303789.05600000004</v>
       </c>
       <c r="AP160">
         <f t="shared" si="69"/>
-        <v>190702785.28</v>
+        <v>26067.52</v>
       </c>
       <c r="AQ160">
         <f t="shared" si="69"/>
-        <v>797574225.5</v>
+        <v>88242.65</v>
       </c>
       <c r="AR160">
         <f t="shared" si="69"/>
-        <v>157499288.09999999</v>
+        <v>13670.118</v>
       </c>
       <c r="AS160">
         <f t="shared" si="69"/>
-        <v>1057748246.16</v>
+        <v>118564.49100000001</v>
       </c>
       <c r="AT160">
         <f t="shared" si="69"/>
-        <v>4644311077.0799999</v>
+        <v>658957.27800000005</v>
       </c>
       <c r="AU160">
         <f t="shared" si="69"/>
-        <v>586696027.5</v>
+        <v>61305.75</v>
       </c>
       <c r="AV160">
         <f t="shared" si="69"/>
-        <v>116443180.38</v>
+        <v>12224.433999999999</v>
       </c>
       <c r="AW160">
         <f t="shared" si="69"/>
-        <v>1759523359.4400001</v>
+        <v>313359.82299999997</v>
       </c>
       <c r="AX160">
         <f t="shared" si="69"/>
-        <v>1571483620</v>
+        <v>259258.58799999996</v>
       </c>
       <c r="AY160">
         <f t="shared" si="69"/>
-        <v>257860976.58000001</v>
+        <v>20450.045999999998</v>
       </c>
       <c r="AZ160">
         <f t="shared" si="69"/>
-        <v>1074461400</v>
+        <v>104880</v>
       </c>
       <c r="BA160">
         <f t="shared" si="69"/>
-        <v>110095891.3</v>
+        <v>9389.42</v>
       </c>
       <c r="BB160">
         <f t="shared" si="69"/>
-        <v>144186257.59999999</v>
+        <v>9054.759</v>
       </c>
     </row>
     <row r="161" spans="1:54" x14ac:dyDescent="0.2">

</xml_diff>